<commit_message>
'Trimowanie' tekstu + poprawka QuickSort-a
</commit_message>
<xml_diff>
--- a/Timesheets/dokumenty/[Fedorowicz, Kamil].xlsx
+++ b/Timesheets/dokumenty/[Fedorowicz, Kamil].xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="Ten_skoroszyt" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="4650" yWindow="0" windowWidth="17640" windowHeight="6750"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="17640" windowHeight="6750"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="33">
   <si>
     <t>Załącznik nr 2</t>
   </si>
@@ -99,31 +99,25 @@
     <t>Ekspert Nadzoru ds. nieruchomości i dostępu do terenu</t>
   </si>
   <si>
-    <t>Przegl?d zawiadomie? o terminie zaj?cia nieruchomo?ci;_x000D_; Sprawdzenie raportu z realizacji Planu Komunikacji;</t>
-  </si>
-  <si>
-    <t>Analiza danych ewidencyjnych;_x000D_; Analiza wzoru umowy z podwykonawcami;</t>
-  </si>
-  <si>
-    <t>Przygotowanie odpowiedzi na pismo PORR ws. dz. nr 2 obr?b Karchowo;_x000D_; Analiza harmonogramu wycinki zieleni;</t>
-  </si>
-  <si>
-    <t>Weryfikacja harmonogramu wycinki;</t>
-  </si>
-  <si>
-    <t>Narada koordynacyjna;_x000D_; Weryfikacja harmonogramu wycinki;</t>
-  </si>
-  <si>
-    <t>Weryfikacja Planu Komunikacji</t>
-  </si>
-  <si>
-    <t>Sprawdzenie Planu Komunikacji i PZJ w zakresie zarz?dzania nieruchomo?ciami;</t>
-  </si>
-  <si>
-    <t>Weryfikacja Protoko?ów z opisania stanu nieruchomo?ci</t>
-  </si>
-  <si>
-    <t>Weryfikacja skrzy?owa? z infrastruktur? techniczn?;_x000D_; Weryfikacja harmonogramu wycinki;</t>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;_x000D_; Przygotowanie do spotkania z właścicielem dz. 1020 obr. Zębowo;</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;_x000D_; Wsparcie WRB w przygotowaniu protokołów przekazania drewna;</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów przekazania drewna;</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;_x000D_; Narada koordynacyjna;</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;_x000D_; Spotkanie z p. Jabłońskich (dot. dz. 106/3 obr. Chmielinko)</t>
+  </si>
+  <si>
+    <t>Weryfikacja protokołów z opisania stanu nieruchomości;_x000D_; Weryfikacja raportu z realizacji planu komunikacji;</t>
   </si>
 </sst>
 </file>
@@ -1286,7 +1280,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="str">
         <f xml:space="preserve"> "Wykaz Czynności nr PS/WC/" &amp; TEXT(C9, "00") &amp; "/" &amp;G9</f>
-        <v>Wykaz Czynności nr PS/WC/02/2017</v>
+        <v>Wykaz Czynności nr PS/WC/05/2017</v>
       </c>
       <c r="B3" s="33"/>
       <c r="C3" s="33"/>
@@ -1360,7 +1354,7 @@
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D9" s="41"/>
       <c r="E9" s="42"/>
@@ -1392,12 +1386,12 @@
       </c>
       <c r="G10" s="44"/>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="45">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B11" s="16">
-        <v>42765</v>
+        <v>42856</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>14</v>
@@ -1407,11 +1401,11 @@
       <c r="F11" s="48"/>
       <c r="G11" s="49"/>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="16">
         <f t="shared" ref="B12:B24" si="0">B11+1</f>
-        <v>42766</v>
+        <v>42857</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>15</v>
@@ -1425,25 +1419,21 @@
       <c r="A13" s="46"/>
       <c r="B13" s="16">
         <f t="shared" si="0"/>
-        <v>42767</v>
+        <v>42858</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="17">
-        <v>1</v>
-      </c>
+      <c r="D13" s="17"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="48" t="s">
-        <v>26</v>
-      </c>
+      <c r="F13" s="48"/>
       <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
       <c r="B14" s="16">
         <f t="shared" si="0"/>
-        <v>42768</v>
+        <v>42859</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>17</v>
@@ -1453,7 +1443,7 @@
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G14" s="49"/>
     </row>
@@ -1461,7 +1451,7 @@
       <c r="A15" s="46"/>
       <c r="B15" s="16">
         <f t="shared" si="0"/>
-        <v>42769</v>
+        <v>42860</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>18</v>
@@ -1471,7 +1461,7 @@
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="48" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G15" s="49"/>
     </row>
@@ -1479,7 +1469,7 @@
       <c r="A16" s="46"/>
       <c r="B16" s="19">
         <f t="shared" si="0"/>
-        <v>42770</v>
+        <v>42861</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>19</v>
@@ -1493,7 +1483,7 @@
       <c r="A17" s="47"/>
       <c r="B17" s="19">
         <f t="shared" si="0"/>
-        <v>42771</v>
+        <v>42862</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>20</v>
@@ -1505,25 +1495,29 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="45">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B18" s="16">
         <f t="shared" si="0"/>
-        <v>42772</v>
+        <v>42863</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="17"/>
+      <c r="D18" s="17">
+        <v>1</v>
+      </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="48"/>
+      <c r="F18" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G18" s="49"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="16">
         <f t="shared" si="0"/>
-        <v>42773</v>
+        <v>42864</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>15</v>
@@ -1533,7 +1527,7 @@
       </c>
       <c r="E19" s="18"/>
       <c r="F19" s="48" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G19" s="49"/>
     </row>
@@ -1541,7 +1535,7 @@
       <c r="A20" s="46"/>
       <c r="B20" s="16">
         <f t="shared" si="0"/>
-        <v>42774</v>
+        <v>42865</v>
       </c>
       <c r="C20" s="16" t="s">
         <v>16</v>
@@ -1551,7 +1545,7 @@
       </c>
       <c r="E20" s="18"/>
       <c r="F20" s="48" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G20" s="49"/>
     </row>
@@ -1559,7 +1553,7 @@
       <c r="A21" s="46"/>
       <c r="B21" s="16">
         <f t="shared" si="0"/>
-        <v>42775</v>
+        <v>42866</v>
       </c>
       <c r="C21" s="16" t="s">
         <v>17</v>
@@ -1569,7 +1563,7 @@
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="48" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G21" s="49"/>
     </row>
@@ -1577,7 +1571,7 @@
       <c r="A22" s="46"/>
       <c r="B22" s="16">
         <f t="shared" si="0"/>
-        <v>42776</v>
+        <v>42867</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>18</v>
@@ -1587,7 +1581,7 @@
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="48" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G22" s="49"/>
     </row>
@@ -1595,7 +1589,7 @@
       <c r="A23" s="46"/>
       <c r="B23" s="19">
         <f t="shared" si="0"/>
-        <v>42777</v>
+        <v>42868</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>19</v>
@@ -1609,7 +1603,7 @@
       <c r="A24" s="47"/>
       <c r="B24" s="19">
         <f t="shared" si="0"/>
-        <v>42778</v>
+        <v>42869</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>20</v>
@@ -1621,11 +1615,11 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="45">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B25" s="16">
         <f>B24+1</f>
-        <v>42779</v>
+        <v>42870</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>14</v>
@@ -1635,7 +1629,7 @@
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="48" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="G25" s="49"/>
     </row>
@@ -1643,7 +1637,7 @@
       <c r="A26" s="46"/>
       <c r="B26" s="16">
         <f t="shared" ref="B26:B45" si="1">B25+1</f>
-        <v>42780</v>
+        <v>42871</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>15</v>
@@ -1653,7 +1647,7 @@
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="48" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="G26" s="49"/>
     </row>
@@ -1661,7 +1655,7 @@
       <c r="A27" s="46"/>
       <c r="B27" s="16">
         <f t="shared" si="1"/>
-        <v>42781</v>
+        <v>42872</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>16</v>
@@ -1671,7 +1665,7 @@
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="48" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G27" s="49"/>
     </row>
@@ -1679,35 +1673,43 @@
       <c r="A28" s="46"/>
       <c r="B28" s="16">
         <f t="shared" si="1"/>
-        <v>42782</v>
+        <v>42873</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="17"/>
+      <c r="D28" s="17">
+        <v>1</v>
+      </c>
       <c r="E28" s="18"/>
-      <c r="F28" s="48"/>
+      <c r="F28" s="48" t="s">
+        <v>29</v>
+      </c>
       <c r="G28" s="49"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="46"/>
       <c r="B29" s="16">
         <f t="shared" si="1"/>
-        <v>42783</v>
+        <v>42874</v>
       </c>
       <c r="C29" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="17">
+        <v>1</v>
+      </c>
       <c r="E29" s="18"/>
-      <c r="F29" s="48"/>
+      <c r="F29" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="46"/>
       <c r="B30" s="19">
         <f t="shared" si="1"/>
-        <v>42784</v>
+        <v>42875</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>19</v>
@@ -1721,7 +1723,7 @@
       <c r="A31" s="47"/>
       <c r="B31" s="19">
         <f t="shared" si="1"/>
-        <v>42785</v>
+        <v>42876</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>20</v>
@@ -1733,81 +1735,101 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="45">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B32" s="16">
         <f t="shared" si="1"/>
-        <v>42786</v>
+        <v>42877</v>
       </c>
       <c r="C32" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="17"/>
+      <c r="D32" s="17">
+        <v>1</v>
+      </c>
       <c r="E32" s="18"/>
-      <c r="F32" s="48"/>
+      <c r="F32" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G32" s="49"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="46"/>
       <c r="B33" s="16">
         <f t="shared" si="1"/>
-        <v>42787</v>
+        <v>42878</v>
       </c>
       <c r="C33" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="17"/>
+      <c r="D33" s="17">
+        <v>1</v>
+      </c>
       <c r="E33" s="18"/>
-      <c r="F33" s="48"/>
+      <c r="F33" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G33" s="49"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="46"/>
       <c r="B34" s="16">
         <f t="shared" si="1"/>
-        <v>42788</v>
+        <v>42879</v>
       </c>
       <c r="C34" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="17"/>
+      <c r="D34" s="17">
+        <v>1</v>
+      </c>
       <c r="E34" s="18"/>
-      <c r="F34" s="48"/>
+      <c r="F34" s="48" t="s">
+        <v>30</v>
+      </c>
       <c r="G34" s="49"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="46"/>
       <c r="B35" s="16">
         <f t="shared" si="1"/>
-        <v>42789</v>
+        <v>42880</v>
       </c>
       <c r="C35" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D35" s="17"/>
+      <c r="D35" s="17">
+        <v>1</v>
+      </c>
       <c r="E35" s="18"/>
-      <c r="F35" s="48"/>
+      <c r="F35" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G35" s="49"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
       <c r="B36" s="16">
         <f t="shared" si="1"/>
-        <v>42790</v>
+        <v>42881</v>
       </c>
       <c r="C36" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="17"/>
+      <c r="D36" s="17">
+        <v>1</v>
+      </c>
       <c r="E36" s="18"/>
-      <c r="F36" s="48"/>
+      <c r="F36" s="48" t="s">
+        <v>26</v>
+      </c>
       <c r="G36" s="49"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
       <c r="B37" s="19">
         <f t="shared" si="1"/>
-        <v>42791</v>
+        <v>42882</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>19</v>
@@ -1821,7 +1843,7 @@
       <c r="A38" s="47"/>
       <c r="B38" s="19">
         <f t="shared" si="1"/>
-        <v>42792</v>
+        <v>42883</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>20</v>
@@ -1833,39 +1855,47 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="45">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="B39" s="16">
         <f t="shared" si="1"/>
-        <v>42793</v>
+        <v>42884</v>
       </c>
       <c r="C39" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="17">
+        <v>1</v>
+      </c>
       <c r="E39" s="18"/>
-      <c r="F39" s="48"/>
+      <c r="F39" s="48" t="s">
+        <v>31</v>
+      </c>
       <c r="G39" s="49"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="46"/>
       <c r="B40" s="16">
         <f t="shared" si="1"/>
-        <v>42794</v>
+        <v>42885</v>
       </c>
       <c r="C40" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="17"/>
+      <c r="D40" s="17">
+        <v>1</v>
+      </c>
       <c r="E40" s="18"/>
-      <c r="F40" s="48"/>
+      <c r="F40" s="48" t="s">
+        <v>32</v>
+      </c>
       <c r="G40" s="49"/>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
       <c r="B41" s="16">
         <f t="shared" si="1"/>
-        <v>42795</v>
+        <v>42886</v>
       </c>
       <c r="C41" s="16" t="s">
         <v>16</v>
@@ -1879,7 +1909,7 @@
       <c r="A42" s="46"/>
       <c r="B42" s="16">
         <f t="shared" si="1"/>
-        <v>42796</v>
+        <v>42887</v>
       </c>
       <c r="C42" s="16" t="s">
         <v>17</v>
@@ -1893,7 +1923,7 @@
       <c r="A43" s="46"/>
       <c r="B43" s="16">
         <f t="shared" si="1"/>
-        <v>42797</v>
+        <v>42888</v>
       </c>
       <c r="C43" s="16" t="s">
         <v>18</v>
@@ -1907,7 +1937,7 @@
       <c r="A44" s="46"/>
       <c r="B44" s="19">
         <f t="shared" si="1"/>
-        <v>42798</v>
+        <v>42889</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>19</v>
@@ -1921,7 +1951,7 @@
       <c r="A45" s="47"/>
       <c r="B45" s="19">
         <f t="shared" si="1"/>
-        <v>42799</v>
+        <v>42890</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>20</v>
@@ -1937,7 +1967,7 @@
         <v>21</v>
       </c>
       <c r="C46" s="25">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D46" s="26"/>
       <c r="E46" s="26"/>

</xml_diff>